<commit_message>
clean-up code and update sensor calibration
</commit_message>
<xml_diff>
--- a/docu/Sharp_IR-Sensoren_Linearisierung.xlsx
+++ b/docu/Sharp_IR-Sensoren_Linearisierung.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\car\docu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53B1DE-67AB-4AB5-BD32-D9385325A62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E327C19E-7474-4997-8E55-F25FAA0AEBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FAD9BF2-B5AE-4568-AE41-C64B5EC617C1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3FAD9BF2-B5AE-4568-AE41-C64B5EC617C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Front" sheetId="1" r:id="rId1"/>
-    <sheet name="Left" sheetId="2" r:id="rId2"/>
-    <sheet name="Right" sheetId="5" r:id="rId3"/>
+    <sheet name="Right" sheetId="5" r:id="rId2"/>
+    <sheet name="Left" sheetId="2" r:id="rId3"/>
     <sheet name="Speedregler" sheetId="3" r:id="rId4"/>
     <sheet name="Spannungsteiler" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Länge</t>
   </si>
@@ -133,6 +133,30 @@
   </si>
   <si>
     <t>Länge l</t>
+  </si>
+  <si>
+    <t>=1/m</t>
+  </si>
+  <si>
+    <t>=m/d</t>
+  </si>
+  <si>
+    <t>y = Wert in Zentimeter</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>x = ADC Wert</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>y = (m'  / (x + d')) - k</t>
+  </si>
+  <si>
+    <t>m'/(ADC + d') - k</t>
   </si>
 </sst>
 </file>
@@ -358,40 +382,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>315</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>125</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,19 +621,64 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>Näherungsgerade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.2747594050743676E-2"/>
-          <c:y val="0.18097222222222226"/>
-          <c:w val="0.85214129483814527"/>
-          <c:h val="0.72125801983085447"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -658,40 +727,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>315</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>125</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,40 +772,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.8461538461538464E-2</c:v>
+                  <c:v>3.7037037037037035E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>2.7027027027027029E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1739130434782608E-2</c:v>
+                  <c:v>2.1276595744680851E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7857142857142856E-2</c:v>
+                  <c:v>1.7543859649122806E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5151515151515152E-2</c:v>
+                  <c:v>1.4925373134328358E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3157894736842105E-2</c:v>
+                  <c:v>1.2987012987012988E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1627906976744186E-2</c:v>
+                  <c:v>1.1494252873563218E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>1.0309278350515464E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.433962264150943E-3</c:v>
+                  <c:v>9.3457943925233638E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6206896551724137E-3</c:v>
+                  <c:v>8.5470085470085479E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.9365079365079361E-3</c:v>
+                  <c:v>7.874015748031496E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.3529411764705881E-3</c:v>
+                  <c:v>7.2992700729927005E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -793,40 +862,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>510</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>405</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>315</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>175</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>155</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>140</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>125</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>95</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,40 +907,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>3.4695867594349561E-2</c:v>
+                  <c:v>3.4594723956935282E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7777777777777773E-2</c:v>
+                  <c:v>2.7027027027027029E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1847986506430526E-2</c:v>
+                  <c:v>2.1270402866669473E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.756535947712418E-2</c:v>
+                  <c:v>1.7001445624157126E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4929896689858738E-2</c:v>
+                  <c:v>1.4414198810513279E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2623866751001474E-2</c:v>
+                  <c:v>1.2732488381644778E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1306135357368751E-2</c:v>
+                  <c:v>1.1180140293458471E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.031783681214421E-2</c:v>
+                  <c:v>1.0339285079024221E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3295382669196687E-3</c:v>
+                  <c:v>9.2397051832255848E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6706725701033091E-3</c:v>
+                  <c:v>8.5928934798146245E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.8800337339236769E-3</c:v>
+                  <c:v>8.075444117085856E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.3529411764705881E-3</c:v>
+                  <c:v>7.2992700729927005E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,6 +1095,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1118,7 +1218,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Left!$B$1</c:f>
+              <c:f>Right!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1153,7 +1253,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Left!$A$2:$A$13</c:f>
+              <c:f>Right!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1186,15 +1286,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Left!$B$2:$B$13</c:f>
+              <c:f>Right!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>185</c:v>
@@ -1203,16 +1303,16 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,7 +1320,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8E41-462F-962B-1395E27DF2D6}"/>
+              <c16:uniqueId val="{00000000-50BF-4DE9-AB5B-041AD3B010A7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1418,19 +1518,64 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>Näherungsgerade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.2747701691844001E-2"/>
-          <c:y val="0.15284265627134161"/>
-          <c:w val="0.85214129483814527"/>
-          <c:h val="0.72125801983085447"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1439,7 +1584,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Left!$C$1</c:f>
+              <c:f>Right!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1474,15 +1619,15 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Left!$B$2:$B$13</c:f>
+              <c:f>Right!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>185</c:v>
@@ -1491,49 +1636,49 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Left!$D$2:$D$13</c:f>
+              <c:f>Right!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.447725503281058E-2</c:v>
+                  <c:v>7.1428571428571425E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.145812479145812E-2</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0162106550995434E-2</c:v>
+                  <c:v>2.9411764705882353E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3210710710710708E-2</c:v>
+                  <c:v>2.2727272727272728E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.8518518518518517E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5911745078411744E-2</c:v>
+                  <c:v>1.5625E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3304971638304972E-2</c:v>
+                  <c:v>1.3513513513513514E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4389945501056624E-3</c:v>
+                  <c:v>1.1904761904761904E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,7 +1686,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C95B-41F4-AFA3-E83DB025B08F}"/>
+              <c16:uniqueId val="{00000000-2EF6-404A-8A7E-5002BF93056F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1550,7 +1695,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Left!$D$1</c:f>
+              <c:f>Right!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1585,15 +1730,15 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Left!$B$2:$B$13</c:f>
+              <c:f>Right!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>185</c:v>
@@ -1602,33 +1747,57 @@
                   <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Left!$E$2:$E$13</c:f>
+              <c:f>Right!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7.322024096635496E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1274435056818472E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7708407889755038E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1873557495319152E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8518518518518517E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5601093321300575E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3121281903665323E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1662569305056351E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C95B-41F4-AFA3-E83DB025B08F}"/>
+              <c16:uniqueId val="{00000001-2EF6-404A-8A7E-5002BF93056F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1775,6 +1944,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1867,7 +2067,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Right!$B$1</c:f>
+              <c:f>Left!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1902,7 +2102,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Right!$A$2:$A$13</c:f>
+              <c:f>Left!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1935,33 +2135,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Right!$B$2:$B$13</c:f>
+              <c:f>Left!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1969,7 +2169,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-50BF-4DE9-AB5B-041AD3B010A7}"/>
+              <c16:uniqueId val="{00000000-8E41-462F-962B-1395E27DF2D6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2167,19 +2367,64 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT"/>
+              <a:t>Näherungsgerade</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="9.2747594050743676E-2"/>
-          <c:y val="0.18097222222222226"/>
-          <c:w val="0.85214129483814527"/>
-          <c:h val="0.72125801983085447"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2188,7 +2433,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Right!$C$1</c:f>
+              <c:f>Left!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2223,43 +2468,43 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Right!$B$2:$B$13</c:f>
+              <c:f>Left!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Right!$C$2:$C$13</c:f>
+              <c:f>Left!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>7.1428571428571425E-2</c:v>
                 </c:pt>
@@ -2290,7 +2535,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-689F-4CBC-8EED-EA5E5204F7D4}"/>
+              <c16:uniqueId val="{00000000-5CB7-489C-80A8-7AC8DA9F9636}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2299,7 +2544,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Right!$D$1</c:f>
+              <c:f>Left!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2334,66 +2579,66 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Right!$B$2:$B$13</c:f>
+              <c:f>Left!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>440</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>185</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>118</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>103</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Right!$D$2:$D$13</c:f>
+              <c:f>Left!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.447725503281058E-2</c:v>
+                  <c:v>7.6978617962224508E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.145812479145812E-2</c:v>
+                  <c:v>4.1287188828172429E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0162106550995434E-2</c:v>
+                  <c:v>3.0364380774216836E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3210710710710708E-2</c:v>
+                  <c:v>2.2826104793317904E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.8518518518518517E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5911745078411744E-2</c:v>
+                  <c:v>1.5441671179376096E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3304971638304972E-2</c:v>
+                  <c:v>1.3134035675019281E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4389945501056624E-3</c:v>
+                  <c:v>1.1595612005448071E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2401,7 +2646,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-689F-4CBC-8EED-EA5E5204F7D4}"/>
+              <c16:uniqueId val="{00000001-5CB7-489C-80A8-7AC8DA9F9636}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2548,6 +2793,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6889,7 +7165,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8CAAF6-27E9-4E63-8140-ED44EDFB12E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688AF597-82B4-4EF0-92CF-59EB2165000D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6911,23 +7187,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>541111</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>377825</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>130810</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>31687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>59552</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+        <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9140CD73-4BDE-429D-B1FA-D0A3334AD4BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7868EB22-3ABD-43D9-8B7B-3866403037FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6970,7 +7246,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{688AF597-82B4-4EF0-92CF-59EB2165000D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8CAAF6-27E9-4E63-8140-ED44EDFB12E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6992,23 +7268,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>541111</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>377825</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>130810</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>16447</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>51932</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagramm 2">
+        <xdr:cNvPr id="5" name="Diagramm 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69E938EE-7BF4-4288-B3F9-6872674932D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74D32D9D-4E7B-4991-A841-0B4D528E589D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7389,10 +7665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDD5582-8EC9-4773-B372-BA84A49938AD}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7401,7 +7677,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -7414,265 +7690,368 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
       <c r="B2" s="6">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C13" si="0">1/(A2+$D$22)</f>
-        <v>3.8461538461538464E-2</v>
+        <f t="shared" ref="C2:C15" si="0">1/(A2+$D$18)</f>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="D2">
-        <f>$D$23*B2+$D$24</f>
-        <v>3.4695867594349561E-2</v>
+        <f t="shared" ref="D2:D15" si="1">$D$19*B2+$D$20</f>
+        <v>3.4594723956935282E-2</v>
+      </c>
+      <c r="E2">
+        <f>$D$21/(B2+$D$22)-$D$18</f>
+        <v>21.906141908946427</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>30</v>
       </c>
       <c r="B3" s="6">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>2.7777777777777776E-2</v>
+        <v>2.7027027027027029E-2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D13" si="1">$D$23*B3+$D$24</f>
-        <v>2.7777777777777773E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="2">$D$21/(B3+$D$22)-$D$18</f>
+        <v>29.999999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40</v>
       </c>
       <c r="B4" s="6">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>2.1739130434782608E-2</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>2.1847986506430526E-2</v>
+        <v>2.1270402866669473E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>40.013684050478936</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>50</v>
       </c>
       <c r="B5" s="6">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>1.7857142857142856E-2</v>
+        <v>1.7543859649122806E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>1.756535947712418E-2</v>
+        <v>1.7001445624157126E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>51.818527677382534</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60</v>
       </c>
       <c r="B6" s="6">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1.5151515151515152E-2</v>
+        <v>1.4925373134328358E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.4929896689858738E-2</v>
+        <v>1.4414198810513279E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>62.376037693515812</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>70</v>
       </c>
       <c r="B7" s="6">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1.3157894736842105E-2</v>
+        <v>1.2987012987012988E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.2623866751001474E-2</v>
+        <v>1.2732488381644778E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>71.539243078486152</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
       <c r="B8" s="6">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.1494252873563218E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1.1306135357368751E-2</v>
+        <v>1.1180140293458471E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>82.44431588082152</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>90</v>
       </c>
       <c r="B9" s="6">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>1.0309278350515464E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>1.031783681214421E-2</v>
+        <v>1.0339285079024221E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>89.718486080700657</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>100</v>
       </c>
       <c r="B10" s="6">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>9.433962264150943E-3</v>
+        <f>1/(A10+$D$18)</f>
+        <v>9.3457943925233638E-3</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>9.3295382669196687E-3</v>
+        <v>9.2397051832255848E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>101.22856142807142</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
       <c r="B11" s="6">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>8.6206896551724137E-3</v>
+        <v>8.5470085470085479E-3</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>8.6706725701033091E-3</v>
+        <v>8.5928934798146245E-3</v>
+      </c>
+      <c r="E11">
+        <f>$D$21/(B11+$D$22)-$D$18</f>
+        <v>109.37523522770041</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>120</v>
       </c>
       <c r="B12" s="6">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>7.9365079365079361E-3</v>
+        <v>7.874015748031496E-3</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>7.8800337339236769E-3</v>
+        <v>8.075444117085856E-3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E15" si="3">$D$21/(B12+$D$22)-$D$18</f>
+        <v>116.83219863836605</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>130</v>
       </c>
       <c r="B13" s="6">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>7.3529411764705881E-3</v>
+        <v>7.2992700729927005E-3</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>7.3529411764705881E-3</v>
+        <v>7.2992700729927005E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>130.00000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>140</v>
       </c>
+      <c r="B14" s="6">
+        <v>82</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>6.8027210884353739E-3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>6.781820710263931E-3</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>140.45302813543159</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>150</v>
       </c>
+      <c r="B15" s="6">
+        <v>78</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>6.369426751592357E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>6.5230960288995467E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>146.30143777887955</v>
+      </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f>(C3-C13)/(B3-B13)</f>
+        <v>6.4681170341096168E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f>C13-(D19*B13)</f>
+        <v>1.4779647422940457E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <f>1/D19</f>
+        <v>15460.449999999997</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="6">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <f>D20/D19</f>
+        <v>22.849999999999973</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <f>(C3-C13)/(B3-B13)</f>
-        <v>6.5886569681636078E-5</v>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <f>C13-(D23*B13)</f>
-        <v>1.0937170567151605E-3</v>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <f>1/D23</f>
-        <v>15177.600000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <f>D24/D23</f>
-        <v>16.600000000000023</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F45B06-3885-459E-8A3A-CD8D9697C8CC}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC3225D-E477-4389-BE20-19943CAF7EFC}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7681,7 +8060,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7694,29 +8073,36 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>440</v>
+        <v>497</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C9" si="0">1/(A2+$D$22)</f>
+        <f t="shared" ref="C2:C9" si="0">1/(A2+$D$18)</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D9" si="1">$D$23*B2+$D$24</f>
-        <v>7.447725503281058E-2</v>
+        <f t="shared" ref="D2:D9" si="1">$D$19*B2+$D$20</f>
+        <v>7.322024096635496E-2</v>
+      </c>
+      <c r="E2">
+        <f>$D$21/(B2+$D$22)-$D$18</f>
+        <v>9.6574256899742341</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
@@ -7724,10 +8110,14 @@
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>4.145812479145812E-2</v>
+        <v>4.1274435056818472E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="2">$D$21/(B3+$D$22)-$D$18</f>
+        <v>20.228072379994977</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -7740,10 +8130,14 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>3.0162106550995434E-2</v>
+        <v>2.7708407889755038E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>32.090128454105148</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
@@ -7756,15 +8150,19 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>2.3210710710710708E-2</v>
+        <v>2.1873557495319152E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>41.717300453481137</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -7774,13 +8172,17 @@
         <f t="shared" si="1"/>
         <v>1.8518518518518517E-2</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -7788,15 +8190,19 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.5911745078411744E-2</v>
+        <v>1.5601093321300575E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>60.098071808510639</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -7804,15 +8210,19 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1.3304971638304972E-2</v>
+        <v>1.3121281903665323E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>72.212065813528341</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -7820,65 +8230,96 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>8.4389945501056624E-3</v>
+        <v>1.1662569305056351E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>81.744399355161491</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f>(C3-C8)/(B3-B8)</f>
+        <v>1.4587125986089715E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f>C6-(D19*B6)</f>
+        <v>7.2222481548906564E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <f>1/D19</f>
+        <v>6855.3600000000006</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <f>D20/D19</f>
+        <v>4.9511111111111212</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <f>(C3-C8)/(B3-B8)</f>
-        <v>1.7378489600711821E-4</v>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <f>C6-(D23*B6)</f>
-        <v>-1.9880992103214305E-3</v>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <f>1/D23</f>
-        <v>5754.2400000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <f>D24/D23</f>
-        <v>-11.439999999999991</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC3225D-E477-4389-BE20-19943CAF7EFC}">
-  <dimension ref="A1:D26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F45B06-3885-459E-8A3A-CD8D9697C8CC}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7887,7 +8328,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7900,29 +8341,36 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>440</v>
+        <v>500</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C9" si="0">1/(A2+$D$22)</f>
+        <f t="shared" ref="C2:C9" si="0">1/(A2+$D$18)</f>
         <v>7.1428571428571425E-2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D9" si="1">$D$23*B2+$D$24</f>
-        <v>7.447725503281058E-2</v>
+        <f t="shared" ref="D2:D9" si="1">$D$19*B2+$D$20</f>
+        <v>7.6978617962224508E-2</v>
+      </c>
+      <c r="E2">
+        <f>$D$21/(B2+$D$22)-$D$18</f>
+        <v>8.99062033681518</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
@@ -7930,15 +8378,19 @@
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
-        <v>4.145812479145812E-2</v>
+        <v>4.1287188828172429E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="2">$D$21/(B3+$D$22)-$D$18</f>
+        <v>20.22058823529412</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
       <c r="B4">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -7946,15 +8398,19 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>3.0162106550995434E-2</v>
+        <v>3.0364380774216836E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>28.933324326150107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>40</v>
       </c>
       <c r="B5">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -7962,15 +8418,19 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>2.3210710710710708E-2</v>
+        <v>2.2826104793317904E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>39.809489575844722</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>50</v>
       </c>
       <c r="B6">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -7980,13 +8440,17 @@
         <f t="shared" si="1"/>
         <v>1.8518518518518517E-2</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>50.000000000000007</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>60</v>
       </c>
       <c r="B7">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -7994,15 +8458,19 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.5911745078411744E-2</v>
+        <v>1.5441671179376096E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>60.759829968119035</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>70</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -8010,15 +8478,19 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1.3304971638304972E-2</v>
+        <v>1.3134035675019281E-2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>72.138060284241774</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>80</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -8026,56 +8498,85 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>8.4389945501056624E-3</v>
+        <v>1.1595612005448071E-2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>82.239518839554222</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <f>(C3-C8)/(B3-B8)</f>
+        <v>1.5384236695712103E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <f>C6-(D19*B6)</f>
+        <v>5.7434483663992841E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <f>1/D19</f>
+        <v>6500.1600000000008</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <f>D20/D19</f>
+        <v>0.37333333333333979</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <f>(C3-C8)/(B3-B8)</f>
-        <v>1.7378489600711821E-4</v>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <f>C6-(D23*B6)</f>
-        <v>-1.9880992103214305E-3</v>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <f>1/D23</f>
-        <v>5754.2400000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <f>D24/D23</f>
-        <v>-11.439999999999991</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8179,7 +8680,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>